<commit_message>
Update database in roles
</commit_message>
<xml_diff>
--- a/Database/MySQL.xlsx
+++ b/Database/MySQL.xlsx
@@ -63,11 +63,6 @@
     <t>FK: users.id</t>
   </si>
   <si>
-    <t>23 ký tự
-Xem thêm
-trong  types.php</t>
-  </si>
-  <si>
     <t>groups</t>
   </si>
   <si>
@@ -248,6 +243,11 @@
   <si>
     <t>Phân loại các tập tin (pdf, 
 img, png,…)</t>
+  </si>
+  <si>
+    <t>23 ký tự
+Xem thêm
+trong  types.php</t>
   </si>
 </sst>
 </file>
@@ -392,9 +392,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -402,6 +399,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,14 +706,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A7" sqref="A7"/>
+      <selection pane="topRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -724,37 +724,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -764,35 +764,29 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -806,81 +800,81 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>59</v>
+      <c r="A5" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -890,34 +884,34 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="14" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -925,125 +919,131 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>64</v>
+      <c r="A15" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>65</v>
+      <c r="A17" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
         <v>39</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
@@ -1053,52 +1053,52 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="7" t="s">
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="E27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename roles -> capabilities, role -> capability
</commit_message>
<xml_diff>
--- a/Database/MySQL.xlsx
+++ b/Database/MySQL.xlsx
@@ -36,9 +36,6 @@
     <t>user_password</t>
   </si>
   <si>
-    <t>role_id</t>
-  </si>
-  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
   </si>
   <si>
     <t>meta_value</t>
-  </si>
-  <si>
-    <t>roles</t>
   </si>
   <si>
     <t>FK: users.id</t>
@@ -119,12 +113,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>user_role</t>
-  </si>
-  <si>
-    <t>FK:roles.id</t>
-  </si>
-  <si>
     <t>banned</t>
   </si>
   <si>
@@ -204,17 +192,6 @@
   </si>
   <si>
     <t>Thông tin mở rộng c.trồng</t>
-  </si>
-  <si>
-    <t>Danh sách các quyền theo
-thứ tự kèm theo tên. Có
-23 roles được định nghĩa
-trong types.php</t>
-  </si>
-  <si>
-    <t>Nếu user A (id=2) có role
-B (id=5) thì cặp (3,5) được 
-lưu vào đây (Đọc types.php) để hiểu kỹ</t>
   </si>
   <si>
     <t>Lưu trữ thông tin nếu như
@@ -248,6 +225,29 @@
     <t>23 ký tự
 Xem thêm
 trong  types.php</t>
+  </si>
+  <si>
+    <t>capabilities</t>
+  </si>
+  <si>
+    <t>user_capability</t>
+  </si>
+  <si>
+    <t>FK:capabilities.id</t>
+  </si>
+  <si>
+    <t>Danh sách các quyền theo
+thứ tự kèm theo tên. Có
+23 capabilities được định 
+nghĩa trong types.php</t>
+  </si>
+  <si>
+    <t>capability_id</t>
+  </si>
+  <si>
+    <t>Nếu user A (id=2) có capability B (id=5) thì cặp
+ (3,5) được lưu vào đây
+(Đọc types.php) để hiểu kỹ</t>
   </si>
 </sst>
 </file>
@@ -706,9 +706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E19" sqref="E19"/>
+      <selection pane="topRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,341 +764,341 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>